<commit_message>
Notes from ODIP meeting and new spreadsheet versio
</commit_message>
<xml_diff>
--- a/WikiFiles/Spray_Seaglider_IMOS_GROOM_Comparison-2013-12-02.xlsx
+++ b/WikiFiles/Spray_Seaglider_IMOS_GROOM_Comparison-2013-12-02.xlsx
@@ -4,55 +4,55 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="15240" windowHeight="7890"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15240" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalAtts" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="odip_updates" sheetId="2" r:id="rId2"/>
+    <sheet name="acdd" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="coverage_content_type" localSheetId="0">GlobalAtts!$C$104</definedName>
-    <definedName name="oovw1245" localSheetId="1">Sheet2!$B$2</definedName>
-    <definedName name="oovw1301" localSheetId="1">Sheet2!$B$4</definedName>
-    <definedName name="oovw1350" localSheetId="1">Sheet2!$B$6</definedName>
-    <definedName name="oovw1404" localSheetId="1">Sheet2!$B$7</definedName>
-    <definedName name="oovw1443" localSheetId="1">Sheet2!$B$8</definedName>
-    <definedName name="oovw1508" localSheetId="1">Sheet2!$B$10</definedName>
-    <definedName name="oovw1554" localSheetId="1">Sheet2!$B$11</definedName>
-    <definedName name="oovw1590" localSheetId="1">Sheet2!$B$12</definedName>
-    <definedName name="oovw1634" localSheetId="1">Sheet2!$B$13</definedName>
-    <definedName name="oovw1715" localSheetId="1">Sheet2!$B$15</definedName>
-    <definedName name="oovw1777" localSheetId="1">Sheet2!$B$16</definedName>
-    <definedName name="oovw1813" localSheetId="1">Sheet2!$B$17</definedName>
-    <definedName name="oovw1842" localSheetId="1">Sheet2!$B$18</definedName>
-    <definedName name="oovw1871" localSheetId="1">Sheet2!$B$19</definedName>
-    <definedName name="oovw1907" localSheetId="1">Sheet2!$B$21</definedName>
-    <definedName name="oovw1969" localSheetId="1">Sheet2!$C$3</definedName>
-    <definedName name="oovw2020" localSheetId="1">Sheet2!$C$4</definedName>
-    <definedName name="oovw2063" localSheetId="1">Sheet2!#REF!</definedName>
-    <definedName name="oovw2086" localSheetId="1">Sheet2!$C$5</definedName>
-    <definedName name="oovw2125" localSheetId="1">Sheet2!$C$6</definedName>
-    <definedName name="oovw2159" localSheetId="1">Sheet2!$C$7</definedName>
-    <definedName name="oovw2193" localSheetId="1">Sheet2!$C$8</definedName>
-    <definedName name="oovw2228" localSheetId="1">Sheet2!$C$9</definedName>
-    <definedName name="oovw2266" localSheetId="1">Sheet2!$C$10</definedName>
-    <definedName name="oovw2296" localSheetId="1">Sheet2!$C$11</definedName>
-    <definedName name="oovw2329" localSheetId="1">Sheet2!#REF!</definedName>
-    <definedName name="oovw2352" localSheetId="1">Sheet2!$C$12</definedName>
-    <definedName name="oovw2383" localSheetId="1">Sheet2!$C$13</definedName>
-    <definedName name="oovw2417" localSheetId="1">Sheet2!#REF!</definedName>
-    <definedName name="oovw2440" localSheetId="1">Sheet2!$C$14</definedName>
-    <definedName name="oovw2472" localSheetId="1">Sheet2!$C$15</definedName>
-    <definedName name="oovw2502" localSheetId="1">Sheet2!$C$16</definedName>
-    <definedName name="oovw2531" localSheetId="1">Sheet2!$C$17</definedName>
-    <definedName name="oovw2567" localSheetId="1">Sheet2!$C$18</definedName>
-    <definedName name="oovw2599" localSheetId="1">Sheet2!#REF!</definedName>
-    <definedName name="oovw2622" localSheetId="1">Sheet2!$B$44</definedName>
+    <definedName name="oovw1245" localSheetId="1">odip_updates!$B$2</definedName>
+    <definedName name="oovw1301" localSheetId="1">odip_updates!$B$4</definedName>
+    <definedName name="oovw1350" localSheetId="1">odip_updates!$B$6</definedName>
+    <definedName name="oovw1404" localSheetId="1">odip_updates!$B$7</definedName>
+    <definedName name="oovw1443" localSheetId="1">odip_updates!$B$8</definedName>
+    <definedName name="oovw1508" localSheetId="1">odip_updates!$B$10</definedName>
+    <definedName name="oovw1554" localSheetId="1">odip_updates!$B$11</definedName>
+    <definedName name="oovw1590" localSheetId="1">odip_updates!$B$12</definedName>
+    <definedName name="oovw1634" localSheetId="1">odip_updates!$B$13</definedName>
+    <definedName name="oovw1715" localSheetId="1">odip_updates!$B$15</definedName>
+    <definedName name="oovw1777" localSheetId="1">odip_updates!$B$16</definedName>
+    <definedName name="oovw1813" localSheetId="1">odip_updates!$B$17</definedName>
+    <definedName name="oovw1842" localSheetId="1">odip_updates!$B$18</definedName>
+    <definedName name="oovw1871" localSheetId="1">odip_updates!$B$19</definedName>
+    <definedName name="oovw1907" localSheetId="1">odip_updates!$B$21</definedName>
+    <definedName name="oovw1969" localSheetId="1">odip_updates!$C$3</definedName>
+    <definedName name="oovw2020" localSheetId="1">odip_updates!$C$4</definedName>
+    <definedName name="oovw2063" localSheetId="1">odip_updates!#REF!</definedName>
+    <definedName name="oovw2086" localSheetId="1">odip_updates!$C$5</definedName>
+    <definedName name="oovw2125" localSheetId="1">odip_updates!$C$6</definedName>
+    <definedName name="oovw2159" localSheetId="1">odip_updates!$C$7</definedName>
+    <definedName name="oovw2193" localSheetId="1">odip_updates!$C$8</definedName>
+    <definedName name="oovw2228" localSheetId="1">odip_updates!$C$9</definedName>
+    <definedName name="oovw2266" localSheetId="1">odip_updates!$C$10</definedName>
+    <definedName name="oovw2296" localSheetId="1">odip_updates!$C$11</definedName>
+    <definedName name="oovw2329" localSheetId="1">odip_updates!#REF!</definedName>
+    <definedName name="oovw2352" localSheetId="1">odip_updates!$C$12</definedName>
+    <definedName name="oovw2383" localSheetId="1">odip_updates!$C$13</definedName>
+    <definedName name="oovw2417" localSheetId="1">odip_updates!#REF!</definedName>
+    <definedName name="oovw2440" localSheetId="1">odip_updates!$C$14</definedName>
+    <definedName name="oovw2472" localSheetId="1">odip_updates!$C$15</definedName>
+    <definedName name="oovw2502" localSheetId="1">odip_updates!$C$16</definedName>
+    <definedName name="oovw2531" localSheetId="1">odip_updates!$C$17</definedName>
+    <definedName name="oovw2567" localSheetId="1">odip_updates!$C$18</definedName>
+    <definedName name="oovw2599" localSheetId="1">odip_updates!#REF!</definedName>
+    <definedName name="oovw2622" localSheetId="1">odip_updates!$B$43</definedName>
     <definedName name="oovw2646" localSheetId="0">GlobalAtts!$Q$34</definedName>
-    <definedName name="oovw2663" localSheetId="1">Sheet2!$B$45</definedName>
-    <definedName name="oovw2693" localSheetId="1">Sheet2!$B$46</definedName>
-    <definedName name="oovw2736" localSheetId="1">Sheet2!$B$47</definedName>
+    <definedName name="oovw2663" localSheetId="1">odip_updates!$B$44</definedName>
+    <definedName name="oovw2693" localSheetId="1">odip_updates!$B$45</definedName>
+    <definedName name="oovw2736" localSheetId="1">odip_updates!$B$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GlobalAtts!$A$1:$Q$107</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GlobalAtts!$2:$4</definedName>
   </definedNames>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="418">
   <si>
     <t>acknowledgment</t>
   </si>
@@ -726,48 +726,15 @@
     <t>contact</t>
   </si>
   <si>
-    <t xml:space="preserve">data_type </t>
-  </si>
-  <si>
-    <t xml:space="preserve">format_version </t>
-  </si>
-  <si>
-    <t xml:space="preserve">platform_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_update </t>
-  </si>
-  <si>
-    <t xml:space="preserve">institution </t>
-  </si>
-  <si>
     <t>institution_edmo_code</t>
   </si>
   <si>
-    <t xml:space="preserve">wmo_platform_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">source </t>
-  </si>
-  <si>
     <t xml:space="preserve">history </t>
   </si>
   <si>
-    <t xml:space="preserve">data_mode </t>
-  </si>
-  <si>
-    <t xml:space="preserve">quality_index </t>
-  </si>
-  <si>
-    <t xml:space="preserve">references </t>
-  </si>
-  <si>
     <t xml:space="preserve">Conventions </t>
   </si>
   <si>
-    <t xml:space="preserve">Netcdf_version </t>
-  </si>
-  <si>
     <t xml:space="preserve">title </t>
   </si>
   <si>
@@ -783,9 +750,6 @@
     <t xml:space="preserve">cdm_data_type </t>
   </si>
   <si>
-    <t xml:space="preserve">area </t>
-  </si>
-  <si>
     <t xml:space="preserve">geospatial_lat_min </t>
   </si>
   <si>
@@ -810,39 +774,6 @@
     <t xml:space="preserve">time_coverage_end </t>
   </si>
   <si>
-    <t xml:space="preserve">institution_references </t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact </t>
-  </si>
-  <si>
-    <t xml:space="preserve">author </t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_assembly_center </t>
-  </si>
-  <si>
-    <t xml:space="preserve">principal_investigator </t>
-  </si>
-  <si>
-    <t>Observatory</t>
-  </si>
-  <si>
-    <t>Deployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distribution_statement </t>
-  </si>
-  <si>
-    <t xml:space="preserve">citation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">update_interval </t>
-  </si>
-  <si>
-    <t xml:space="preserve">qc_manual </t>
-  </si>
-  <si>
     <t>data_assembly_centre</t>
   </si>
   <si>
@@ -1192,6 +1123,198 @@
   </si>
   <si>
     <t>Recomended if data go to GTS.  Reconcile with wmo_id and usage corresponding to platform container variables.</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>acknowledgement</t>
+  </si>
+  <si>
+    <t>http://wiki.esipfed.org/index.php/Attribute_Convention_for_Data_Discovery_%28ACDD%29</t>
+  </si>
+  <si>
+    <t>http://wiki.esipfed.org/index.php/Attribute_Convention_for_Data_Discovery_%28ACDD%29_Working</t>
+  </si>
+  <si>
+    <t>ioos</t>
+  </si>
+  <si>
+    <t>imos</t>
+  </si>
+  <si>
+    <t>ego</t>
+  </si>
+  <si>
+    <t>acdd (Current v.1.1.1)</t>
+  </si>
+  <si>
+    <t>acdd (Working v.1.2beta)</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acknowledgement </t>
+  </si>
+  <si>
+    <t>Use ACDD creator instead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment </t>
+  </si>
+  <si>
+    <t>Use other roles from ACDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contributor_info </t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverage_content_type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator_email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator_uri </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator_institution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator_institution_info </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator_project </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator_project_info </t>
+  </si>
+  <si>
+    <t>data_assembly_center</t>
+  </si>
+  <si>
+    <t>Use data_assembly_center</t>
+  </si>
+  <si>
+    <t>Create reference vocabulary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_created </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_modified </t>
+  </si>
+  <si>
+    <t>Use date_modified</t>
+  </si>
+  <si>
+    <t>Use license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_bounds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_lat_resolution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_lat_units </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_lon_resolution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_lon_units </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_vertical_positive </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_vertical_resolution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geospatial_vertical_units </t>
+  </si>
+  <si>
+    <t>Use instrument variable instead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywords </t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywords_vocabulary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">license </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metadata_Convention </t>
+  </si>
+  <si>
+    <t xml:space="preserve">metadata_link </t>
+  </si>
+  <si>
+    <t>Use platform container variable instead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">processing_level </t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher_email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher_institution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher_institution_info </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher_project </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher_project_info </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher_uri </t>
+  </si>
+  <si>
+    <t>Use publisher instead</t>
+  </si>
+  <si>
+    <t>Use publisher_uri instead</t>
+  </si>
+  <si>
+    <t>qc_manual (or qc_reference?)</t>
+  </si>
+  <si>
+    <t>??? Meaning is good, not sure if this is the best term</t>
+  </si>
+  <si>
+    <t>None, many other references already exist</t>
+  </si>
+  <si>
+    <t>Use area instead?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time_coverage_duration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">time_coverage_resolution </t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1331,6 +1454,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1341,7 +1479,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1431,6 +1569,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1440,73 +1588,9 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1557,6 +1641,77 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1894,13 +2049,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1912,28 +2060,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:Q97" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:Q97" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="A4:Q97"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="IOOS Recommendation" dataDxfId="16"/>
-    <tableColumn id="2" name="Is CF (Y/N)" dataDxfId="15"/>
-    <tableColumn id="3" name="Is ACDD (Y/N)" dataDxfId="14"/>
-    <tableColumn id="4" name="Is IMOS (Y/N)" dataDxfId="13">
+    <tableColumn id="1" name="IOOS Recommendation" dataDxfId="17"/>
+    <tableColumn id="2" name="Is CF (Y/N)" dataDxfId="16"/>
+    <tableColumn id="3" name="Is ACDD (Y/N)" dataDxfId="15"/>
+    <tableColumn id="4" name="Is IMOS (Y/N)" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(L5),"","y")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Is EGO (Y/N)2" dataDxfId="12"/>
-    <tableColumn id="5" name="Global Attribute" dataDxfId="11"/>
-    <tableColumn id="6" name="Attribute Value (example)" dataDxfId="10"/>
-    <tableColumn id="7" name="Comments" dataDxfId="9"/>
-    <tableColumn id="8" name="Global Attribute2" dataDxfId="8"/>
-    <tableColumn id="9" name="Attribute Value (example)2" dataDxfId="7"/>
-    <tableColumn id="10" name="Comments2" dataDxfId="6"/>
-    <tableColumn id="11" name="Global Attribute3" dataDxfId="2"/>
-    <tableColumn id="12" name="Attribute Value (example)3" dataDxfId="0"/>
-    <tableColumn id="17" name="Comments3" dataDxfId="1"/>
-    <tableColumn id="14" name="Global Attribute4" dataDxfId="5"/>
-    <tableColumn id="15" name="Attribute Value (example)4" dataDxfId="4"/>
-    <tableColumn id="16" name="Comments4" dataDxfId="3"/>
+    <tableColumn id="18" name="Is EGO (Y/N)2" dataDxfId="13"/>
+    <tableColumn id="5" name="Global Attribute" dataDxfId="12"/>
+    <tableColumn id="6" name="Attribute Value (example)" dataDxfId="11"/>
+    <tableColumn id="7" name="Comments" dataDxfId="10"/>
+    <tableColumn id="8" name="Global Attribute2" dataDxfId="9"/>
+    <tableColumn id="9" name="Attribute Value (example)2" dataDxfId="8"/>
+    <tableColumn id="10" name="Comments2" dataDxfId="7"/>
+    <tableColumn id="11" name="Global Attribute3" dataDxfId="6"/>
+    <tableColumn id="12" name="Attribute Value (example)3" dataDxfId="5"/>
+    <tableColumn id="17" name="Comments3" dataDxfId="4"/>
+    <tableColumn id="14" name="Global Attribute4" dataDxfId="3"/>
+    <tableColumn id="15" name="Attribute Value (example)4" dataDxfId="2"/>
+    <tableColumn id="16" name="Comments4" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2231,8 +2379,8 @@
   </sheetPr>
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,7 +2454,7 @@
     </row>
     <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>154</v>
@@ -2318,7 +2466,7 @@
         <v>143</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>108</v>
@@ -2348,18 +2496,18 @@
         <v>219</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="P4" s="26" t="s">
         <v>218</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -2388,15 +2536,15 @@
         <v>156</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="Q5" s="27" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="3" t="s">
@@ -2425,7 +2573,7 @@
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="19" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>158</v>
@@ -2437,7 +2585,7 @@
     </row>
     <row r="7" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="3"/>
@@ -2458,18 +2606,18 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="19" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="3"/>
@@ -2498,15 +2646,15 @@
         <v>159</v>
       </c>
       <c r="P8" s="27" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="Q8" s="27" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="3"/>
@@ -2636,10 +2784,10 @@
         <v>2</v>
       </c>
       <c r="P12" s="27" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -2674,7 +2822,7 @@
       </c>
       <c r="P13" s="27"/>
       <c r="Q13" s="27" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="135" x14ac:dyDescent="0.25">
@@ -2714,15 +2862,15 @@
         <v>4</v>
       </c>
       <c r="P14" s="27" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="3"/>
@@ -2746,10 +2894,10 @@
         <v>220</v>
       </c>
       <c r="P15" s="31" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -2857,10 +3005,10 @@
         <v>166</v>
       </c>
       <c r="P18" s="27" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="Q18" s="27" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -2973,7 +3121,7 @@
     </row>
     <row r="22" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="3"/>
@@ -2994,13 +3142,13 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="19" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="P22" s="18" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3067,7 +3215,7 @@
     </row>
     <row r="25" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="3"/>
@@ -3088,18 +3236,18 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="19" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="P25" s="18" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="Q25" s="10" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="3"/>
@@ -3120,13 +3268,13 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="19" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3174,7 +3322,7 @@
     </row>
     <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="3" t="s">
@@ -3208,7 +3356,7 @@
     </row>
     <row r="29" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="3" t="s">
@@ -3246,7 +3394,7 @@
     </row>
     <row r="30" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="3"/>
@@ -3267,13 +3415,13 @@
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
       <c r="O30" s="19" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="P30" s="18" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -3297,13 +3445,13 @@
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
       <c r="O31" s="19" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="P31" s="18" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="Q31" s="10" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3367,10 +3515,10 @@
         <v>173</v>
       </c>
       <c r="P33" s="31" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="Q33" s="29" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3472,7 +3620,7 @@
     </row>
     <row r="37" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="3"/>
@@ -3493,18 +3641,18 @@
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="19" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="P37" s="18" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="Q37" s="10" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="3" t="s">
@@ -3544,12 +3692,12 @@
       </c>
       <c r="P38" s="27"/>
       <c r="Q38" s="27" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="3" t="s">
@@ -3589,12 +3737,12 @@
       </c>
       <c r="P39" s="27"/>
       <c r="Q39" s="27" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="3" t="s">
@@ -3631,7 +3779,7 @@
     </row>
     <row r="41" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="3" t="s">
@@ -3668,7 +3816,7 @@
     </row>
     <row r="42" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="3" t="s">
@@ -3708,12 +3856,12 @@
       </c>
       <c r="P42" s="27"/>
       <c r="Q42" s="27" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="3" t="s">
@@ -3753,12 +3901,12 @@
       </c>
       <c r="P43" s="27"/>
       <c r="Q43" s="27" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="3" t="s">
@@ -3795,7 +3943,7 @@
     </row>
     <row r="45" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="3" t="s">
@@ -3832,7 +3980,7 @@
     </row>
     <row r="46" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="3" t="s">
@@ -3872,12 +4020,12 @@
       </c>
       <c r="P46" s="27"/>
       <c r="Q46" s="27" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="3" t="s">
@@ -3917,12 +4065,12 @@
       </c>
       <c r="P47" s="27"/>
       <c r="Q47" s="27" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="3" t="s">
@@ -3961,7 +4109,7 @@
     </row>
     <row r="49" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="3" t="s">
@@ -4000,7 +4148,7 @@
     </row>
     <row r="50" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="3" t="s">
@@ -4037,7 +4185,7 @@
     </row>
     <row r="51" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="3"/>
@@ -4109,15 +4257,15 @@
         <v>52</v>
       </c>
       <c r="P52" s="27" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="Q52" s="28" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="3"/>
@@ -4138,18 +4286,18 @@
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
       <c r="O53" s="19" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="P53" s="18" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="Q53" s="27" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="3" t="s">
@@ -4184,7 +4332,7 @@
         <v>53</v>
       </c>
       <c r="P54" s="18" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
       <c r="Q54" s="27"/>
     </row>
@@ -4229,15 +4377,15 @@
         <v>55</v>
       </c>
       <c r="P55" s="27" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="Q55" s="27" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="3"/>
@@ -4258,13 +4406,13 @@
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
       <c r="O56" s="19" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="P56" s="18" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="Q56" s="10" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -4295,15 +4443,15 @@
         <v>177</v>
       </c>
       <c r="P57" s="32" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="Q57" s="27" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="3"/>
@@ -4378,10 +4526,10 @@
         <v>58</v>
       </c>
       <c r="P59" s="27" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="Q59" s="27" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -4624,10 +4772,10 @@
         <v>67</v>
       </c>
       <c r="P66" s="27" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="Q66" s="28" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -4651,13 +4799,13 @@
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
       <c r="O67" s="19" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="P67" s="18" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="Q67" s="10" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -4711,13 +4859,13 @@
       <c r="M69" s="10"/>
       <c r="N69" s="10"/>
       <c r="O69" s="19" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="P69" s="18" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="Q69" s="10" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -4756,7 +4904,7 @@
     </row>
     <row r="71" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="3"/>
@@ -4785,15 +4933,15 @@
         <v>182</v>
       </c>
       <c r="P71" s="27" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="Q71" s="27" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="B72" s="9"/>
       <c r="C72" s="3"/>
@@ -4890,10 +5038,10 @@
         <v>184</v>
       </c>
       <c r="P74" s="27" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="Q74" s="27" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -4927,10 +5075,10 @@
         <v>186</v>
       </c>
       <c r="P75" s="32" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="Q75" s="27" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -5084,7 +5232,7 @@
     </row>
     <row r="80" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="3"/>
@@ -5105,18 +5253,18 @@
       <c r="M80" s="10"/>
       <c r="N80" s="10"/>
       <c r="O80" s="19" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="P80" s="32" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="Q80" s="10" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="3"/>
@@ -5146,7 +5294,7 @@
     </row>
     <row r="82" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="3"/>
@@ -5177,7 +5325,7 @@
     </row>
     <row r="83" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="3"/>
@@ -5198,13 +5346,13 @@
       <c r="M83" s="10"/>
       <c r="N83" s="10"/>
       <c r="O83" s="19" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="P83" s="18" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
       <c r="Q83" s="10" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="135" x14ac:dyDescent="0.25">
@@ -5248,15 +5396,15 @@
         <v>84</v>
       </c>
       <c r="P84" s="32" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
       <c r="Q84" s="27" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="3"/>
@@ -5320,7 +5468,7 @@
     </row>
     <row r="87" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>151</v>
@@ -5359,10 +5507,10 @@
         <v>89</v>
       </c>
       <c r="P87" s="27" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
       <c r="Q87" s="27" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -5469,10 +5617,10 @@
         <v>93</v>
       </c>
       <c r="P90" s="27" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
       <c r="Q90" s="27" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="60" x14ac:dyDescent="0.25">
@@ -5516,10 +5664,10 @@
         <v>95</v>
       </c>
       <c r="P91" s="27" t="s">
-        <v>349</v>
+        <v>326</v>
       </c>
       <c r="Q91" s="27" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
@@ -5600,10 +5748,10 @@
         <v>99</v>
       </c>
       <c r="P93" s="27" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
       <c r="Q93" s="18" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="135" x14ac:dyDescent="0.25">
@@ -5649,15 +5797,15 @@
         <v>101</v>
       </c>
       <c r="P94" s="27" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
       <c r="Q94" s="10" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
     </row>
     <row r="95" spans="1:17" s="24" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="3"/>
@@ -5679,13 +5827,13 @@
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
       <c r="O95" s="19" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="P95" s="18" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
       <c r="Q95" s="4" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="60" x14ac:dyDescent="0.25">
@@ -5725,7 +5873,7 @@
     </row>
     <row r="97" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A97" s="25" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5747,13 +5895,13 @@
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
       <c r="O97" s="1" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="P97" s="25" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="Q97" s="4" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -6010,7 +6158,7 @@
     <mergeCell ref="L3:N3"/>
   </mergeCells>
   <conditionalFormatting sqref="O93 O42:O43 O46:O47 O57 O59 O66:O67 O71 O74:O75 O84 O91 L93:L97 L5:L91 I5:I97 F5:F97">
-    <cfRule type="containsBlanks" dxfId="20" priority="18" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6033,10 +6181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C22"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6045,177 +6193,1447 @@
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>366</v>
+      </c>
+      <c r="G9" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>368</v>
+      </c>
+      <c r="G11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" t="s">
+        <v>223</v>
+      </c>
+      <c r="G14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>370</v>
+      </c>
+      <c r="G15" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>371</v>
+      </c>
+      <c r="G16" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>372</v>
+      </c>
+      <c r="G17" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>373</v>
+      </c>
+      <c r="G18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>374</v>
+      </c>
+      <c r="G19" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>375</v>
+      </c>
+      <c r="G20" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>376</v>
+      </c>
+      <c r="G21" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>377</v>
+      </c>
+      <c r="G22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>237</v>
+      </c>
+      <c r="G23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G24" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="G26" t="s">
+        <v>238</v>
+      </c>
+      <c r="H26" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>239</v>
+      </c>
+      <c r="G27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>381</v>
+      </c>
+      <c r="G28" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>383</v>
+      </c>
+      <c r="G30" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
         <v>240</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G31" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" t="s">
+        <v>386</v>
+      </c>
+      <c r="G36" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>230</v>
+      </c>
+      <c r="G37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" t="s">
+        <v>229</v>
+      </c>
+      <c r="G38" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>387</v>
+      </c>
+      <c r="G39" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" t="s">
+        <v>388</v>
+      </c>
+      <c r="G40" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" t="s">
+        <v>232</v>
+      </c>
+      <c r="G41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" t="s">
+        <v>231</v>
+      </c>
+      <c r="G42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>389</v>
+      </c>
+      <c r="G43" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" t="s">
+        <v>390</v>
+      </c>
+      <c r="G44" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>233</v>
+      </c>
+      <c r="G46" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>391</v>
+      </c>
+      <c r="G47" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
+        <v>392</v>
+      </c>
+      <c r="G48" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>393</v>
+      </c>
+      <c r="G49" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
+        <v>222</v>
+      </c>
+      <c r="G50" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="D51" t="s">
+        <v>250</v>
+      </c>
+      <c r="G51" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" t="s">
+        <v>227</v>
+      </c>
+      <c r="G52" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E53" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="D54" t="s">
+        <v>221</v>
+      </c>
+      <c r="G54" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
+        <v>177</v>
+      </c>
+      <c r="D55" t="s">
+        <v>177</v>
+      </c>
+      <c r="G55" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="G56" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F57" t="s">
+        <v>395</v>
+      </c>
+      <c r="G57" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" t="s">
+        <v>396</v>
+      </c>
+      <c r="G58" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="C59" t="s">
+        <v>180</v>
+      </c>
+      <c r="G59" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+      <c r="E60" t="s">
+        <v>62</v>
+      </c>
+      <c r="F60" t="s">
+        <v>397</v>
+      </c>
+      <c r="G60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="F61" t="s">
+        <v>398</v>
+      </c>
+      <c r="G61" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" t="s">
+        <v>399</v>
+      </c>
+      <c r="G62" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" t="s">
+        <v>67</v>
+      </c>
+      <c r="F63" t="s">
+        <v>226</v>
+      </c>
+      <c r="G63" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="D64" t="s">
+        <v>242</v>
+      </c>
+      <c r="G64" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>243</v>
+      </c>
+      <c r="G65" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>71</v>
+      </c>
+      <c r="G66" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s">
+        <v>182</v>
+      </c>
+      <c r="D67" t="s">
+        <v>182</v>
+      </c>
+      <c r="G67" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="E68" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" t="s">
+        <v>401</v>
+      </c>
+      <c r="G68" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="C69" t="s">
+        <v>184</v>
+      </c>
+      <c r="D69" t="s">
+        <v>184</v>
+      </c>
+      <c r="G69" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>71</v>
+      </c>
+      <c r="C70" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" t="s">
+        <v>186</v>
+      </c>
+      <c r="G70" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" t="s">
+        <v>75</v>
+      </c>
+      <c r="G71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>73</v>
+      </c>
+      <c r="F72" t="s">
+        <v>403</v>
+      </c>
+      <c r="G72" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>74</v>
+      </c>
+      <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" t="s">
+        <v>77</v>
+      </c>
+      <c r="F73" t="s">
+        <v>404</v>
+      </c>
+      <c r="G73" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>75</v>
+      </c>
+      <c r="F74" t="s">
+        <v>405</v>
+      </c>
+      <c r="G74" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>76</v>
+      </c>
+      <c r="F75" t="s">
+        <v>406</v>
+      </c>
+      <c r="G75" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>77</v>
+      </c>
+      <c r="F76" t="s">
+        <v>407</v>
+      </c>
+      <c r="G76" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>78</v>
+      </c>
+      <c r="F77" t="s">
+        <v>408</v>
+      </c>
+      <c r="G77" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>80</v>
+      </c>
+      <c r="F78" t="s">
+        <v>409</v>
+      </c>
+      <c r="G78" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>81</v>
+      </c>
+      <c r="B79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E79" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="G80" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>83</v>
+      </c>
+      <c r="D81" t="s">
+        <v>246</v>
+      </c>
+      <c r="G81" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>189</v>
+      </c>
+      <c r="G82" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>86</v>
+      </c>
+      <c r="D83" t="s">
+        <v>247</v>
+      </c>
+      <c r="G83" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>88</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" t="s">
+        <v>84</v>
+      </c>
+      <c r="D84" t="s">
+        <v>84</v>
+      </c>
+      <c r="G84" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>89</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+      <c r="G85" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>90</v>
+      </c>
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>89</v>
+      </c>
+      <c r="D86" t="s">
+        <v>89</v>
+      </c>
+      <c r="G86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>91</v>
+      </c>
+      <c r="B87" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" t="s">
+        <v>91</v>
+      </c>
+      <c r="G87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>92</v>
+      </c>
+      <c r="B88" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" t="s">
+        <v>93</v>
+      </c>
+      <c r="E88" t="s">
+        <v>93</v>
+      </c>
+      <c r="F88" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>239</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G88" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>93</v>
+      </c>
+      <c r="E89" t="s">
+        <v>153</v>
+      </c>
+      <c r="F89" t="s">
+        <v>416</v>
+      </c>
+      <c r="G89" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>94</v>
+      </c>
+      <c r="B90" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90" t="s">
+        <v>95</v>
+      </c>
+      <c r="D90" t="s">
+        <v>95</v>
+      </c>
+      <c r="E90" t="s">
+        <v>95</v>
+      </c>
+      <c r="F90" t="s">
+        <v>236</v>
+      </c>
+      <c r="G90" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>95</v>
+      </c>
+      <c r="B91" t="s">
+        <v>97</v>
+      </c>
+      <c r="E91" t="s">
+        <v>97</v>
+      </c>
+      <c r="F91" t="s">
+        <v>417</v>
+      </c>
+      <c r="G91" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>96</v>
+      </c>
+      <c r="B92" t="s">
+        <v>99</v>
+      </c>
+      <c r="C92" t="s">
+        <v>99</v>
+      </c>
+      <c r="D92" t="s">
+        <v>99</v>
+      </c>
+      <c r="E92" t="s">
+        <v>99</v>
+      </c>
+      <c r="F92" t="s">
+        <v>235</v>
+      </c>
+      <c r="G92" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>97</v>
+      </c>
+      <c r="B93" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" t="s">
+        <v>101</v>
+      </c>
+      <c r="E93" t="s">
+        <v>101</v>
+      </c>
+      <c r="F93" t="s">
+        <v>224</v>
+      </c>
+      <c r="G93" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>97</v>
+      </c>
+      <c r="D94" t="s">
+        <v>248</v>
+      </c>
+      <c r="G94" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>97</v>
+      </c>
+      <c r="B95" t="s">
+        <v>103</v>
+      </c>
+      <c r="G95" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>97</v>
+      </c>
+      <c r="D96" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>230</v>
-      </c>
-      <c r="C10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>224</v>
-      </c>
-      <c r="C12" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>255</v>
-      </c>
-      <c r="C13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>256</v>
-      </c>
-      <c r="C14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>222</v>
-      </c>
-      <c r="C15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C16" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>241</v>
-      </c>
-      <c r="C17" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>243</v>
-      </c>
-      <c r="C19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>246</v>
-      </c>
-      <c r="C20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>245</v>
-      </c>
-      <c r="C21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>229</v>
+      <c r="G96" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -6229,12 +7647,241 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>